<commit_message>
DA 20 | Day_1
</commit_message>
<xml_diff>
--- a/Batch/19/Day_1.xlsx
+++ b/Batch/19/Day_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29115"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive\Work\Acciojob\Modules\Excel\Batch\19\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive\Work\Acciojob\Modules\excel\Batch\19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093983A3-FFF9-4B29-9AA2-4FB1D674AAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA38EEA-A29C-4BA3-8170-D02EA0AB78DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -3215,24 +3215,9 @@
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3249,12 +3234,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3265,6 +3244,27 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -3550,6 +3550,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -3557,7 +3558,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4874,8 +4874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:M44"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41:M42"/>
+    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5246,7 +5246,7 @@
       <c r="F38" t="s">
         <v>21</v>
       </c>
-      <c r="I38" s="1" t="s">
+      <c r="I38" s="16" t="s">
         <v>21</v>
       </c>
     </row>
@@ -5263,14 +5263,14 @@
       <c r="H39" t="s">
         <v>42</v>
       </c>
-      <c r="I39" s="1"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="3" t="s">
+      <c r="I39" s="16"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="17" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="40" spans="2:13">
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="18" t="s">
         <v>46</v>
       </c>
       <c r="D40" t="s">
@@ -5285,30 +5285,30 @@
       <c r="H40" t="s">
         <v>45</v>
       </c>
-      <c r="I40" s="1"/>
-      <c r="K40" s="3"/>
+      <c r="I40" s="16"/>
+      <c r="K40" s="17"/>
     </row>
     <row r="41" spans="2:13">
-      <c r="B41" s="4"/>
+      <c r="B41" s="18"/>
       <c r="D41" t="s">
         <v>38</v>
       </c>
-      <c r="J41" s="2"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="4" t="s">
+      <c r="J41" s="1"/>
+      <c r="K41" s="17"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="18" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="42" spans="2:13">
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L42" s="5"/>
-      <c r="M42" s="4"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="18"/>
     </row>
     <row r="43" spans="2:13">
       <c r="D43" t="s">
@@ -5346,8 +5346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{766E4D3D-83B2-4B91-A055-E6D373754FAF}">
   <dimension ref="B2:M338"/>
   <sheetViews>
-    <sheetView topLeftCell="A275" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I291" sqref="I291"/>
+    <sheetView topLeftCell="A28" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B338" sqref="B36:M338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5362,13 +5362,13 @@
       </c>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" t="s">
@@ -5376,11 +5376,11 @@
       </c>
     </row>
     <row r="33" spans="2:13">
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
       <c r="F33" t="s">
         <v>47</v>
       </c>
@@ -5389,123 +5389,123 @@
       <c r="B36" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="19"/>
     </row>
     <row r="37" spans="2:13">
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19"/>
     </row>
     <row r="38" spans="2:13">
       <c r="B38" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
-      <c r="L38" s="9"/>
-      <c r="M38" s="9"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="21"/>
     </row>
     <row r="39" spans="2:13">
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
-      <c r="L39" s="9"/>
-      <c r="M39" s="9"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="21"/>
     </row>
     <row r="40" spans="2:13">
       <c r="B40" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
-      <c r="M40" s="8"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
     </row>
     <row r="41" spans="2:13">
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
-      <c r="M41" s="8"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="19"/>
     </row>
     <row r="42" spans="2:13">
       <c r="B42" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="8"/>
-      <c r="M42" s="8"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="19"/>
     </row>
     <row r="43" spans="2:13">
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="8"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="19"/>
+      <c r="M43" s="19"/>
     </row>
     <row r="47" spans="2:13">
       <c r="B47" t="s">
@@ -5565,7 +5565,7 @@
       <c r="B53" t="s">
         <v>56</v>
       </c>
-      <c r="E53" s="5" t="s">
+      <c r="E53" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F53" t="s">
@@ -5582,7 +5582,7 @@
       <c r="B54" t="s">
         <v>59</v>
       </c>
-      <c r="E54" s="5" t="s">
+      <c r="E54" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F54" t="s">
@@ -5599,7 +5599,7 @@
       <c r="B55" t="s">
         <v>23</v>
       </c>
-      <c r="E55" s="5" t="s">
+      <c r="E55" s="2" t="s">
         <v>60</v>
       </c>
       <c r="G55" t="s">
@@ -5632,7 +5632,7 @@
       <c r="B58" t="s">
         <v>66</v>
       </c>
-      <c r="E58" s="5" t="s">
+      <c r="E58" s="2" t="s">
         <v>67</v>
       </c>
     </row>
@@ -5657,86 +5657,86 @@
       </c>
     </row>
     <row r="64" spans="2:9" ht="17.649999999999999">
-      <c r="B64" s="10" t="s">
+      <c r="B64" s="5" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="65" spans="2:2">
-      <c r="B65" s="11"/>
+      <c r="B65" s="6"/>
     </row>
     <row r="66" spans="2:2">
-      <c r="B66" s="12" t="s">
+      <c r="B66" s="7" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="67" spans="2:2">
-      <c r="B67" s="12" t="s">
+      <c r="B67" s="7" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="68" spans="2:2">
-      <c r="B68" s="12" t="s">
+      <c r="B68" s="7" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="70" spans="2:2" ht="17.649999999999999">
-      <c r="B70" s="10" t="s">
+      <c r="B70" s="5" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="71" spans="2:2">
-      <c r="B71" s="11"/>
+      <c r="B71" s="6"/>
     </row>
     <row r="72" spans="2:2">
-      <c r="B72" s="12" t="s">
+      <c r="B72" s="7" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="73" spans="2:2">
-      <c r="B73" s="12" t="s">
+      <c r="B73" s="7" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="74" spans="2:2">
-      <c r="B74" s="12" t="s">
+      <c r="B74" s="7" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="75" spans="2:2">
-      <c r="B75" s="12" t="s">
+      <c r="B75" s="7" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="77" spans="2:2" ht="17.649999999999999">
-      <c r="B77" s="10" t="s">
+      <c r="B77" s="5" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="78" spans="2:2">
-      <c r="B78" s="11"/>
+      <c r="B78" s="6"/>
     </row>
     <row r="79" spans="2:2">
-      <c r="B79" s="12" t="s">
+      <c r="B79" s="7" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="80" spans="2:2">
-      <c r="B80" s="12" t="s">
+      <c r="B80" s="7" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="81" spans="2:2">
-      <c r="B81" s="12" t="s">
+      <c r="B81" s="7" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="82" spans="2:2">
-      <c r="B82" s="12" t="s">
+      <c r="B82" s="7" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="86" spans="2:2" ht="17.649999999999999">
-      <c r="B86" s="10" t="s">
+      <c r="B86" s="5" t="s">
         <v>85</v>
       </c>
     </row>
@@ -5746,241 +5746,241 @@
       </c>
     </row>
     <row r="90" spans="2:2" ht="15.75">
-      <c r="B90" s="13" t="s">
+      <c r="B90" s="8" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="91" spans="2:2">
-      <c r="B91" s="11"/>
+      <c r="B91" s="6"/>
     </row>
     <row r="92" spans="2:2">
-      <c r="B92" s="12" t="s">
+      <c r="B92" s="7" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="93" spans="2:2">
-      <c r="B93" s="12" t="s">
+      <c r="B93" s="7" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="94" spans="2:2">
-      <c r="B94" s="12" t="s">
+      <c r="B94" s="7" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="95" spans="2:2">
-      <c r="B95" s="12" t="s">
+      <c r="B95" s="7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="97" spans="2:2" ht="15.75">
-      <c r="B97" s="13" t="s">
+      <c r="B97" s="8" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="98" spans="2:2">
-      <c r="B98" s="11"/>
+      <c r="B98" s="6"/>
     </row>
     <row r="99" spans="2:2">
-      <c r="B99" s="12" t="s">
+      <c r="B99" s="7" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="100" spans="2:2">
-      <c r="B100" s="12" t="s">
+      <c r="B100" s="7" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="101" spans="2:2">
-      <c r="B101" s="12" t="s">
+      <c r="B101" s="7" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="102" spans="2:2">
-      <c r="B102" s="12" t="s">
+      <c r="B102" s="7" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="104" spans="2:2" ht="15.75">
-      <c r="B104" s="13" t="s">
+      <c r="B104" s="8" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="105" spans="2:2">
-      <c r="B105" s="11"/>
+      <c r="B105" s="6"/>
     </row>
     <row r="106" spans="2:2">
-      <c r="B106" s="12" t="s">
+      <c r="B106" s="7" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="107" spans="2:2">
-      <c r="B107" s="12" t="s">
+      <c r="B107" s="7" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="108" spans="2:2">
-      <c r="B108" s="12" t="s">
+      <c r="B108" s="7" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="109" spans="2:2">
-      <c r="B109" s="12" t="s">
+      <c r="B109" s="7" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="111" spans="2:2" ht="15.75">
-      <c r="B111" s="13" t="s">
+      <c r="B111" s="8" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="112" spans="2:2">
-      <c r="B112" s="11"/>
+      <c r="B112" s="6"/>
     </row>
     <row r="113" spans="2:2">
-      <c r="B113" s="12" t="s">
+      <c r="B113" s="7" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="114" spans="2:2">
-      <c r="B114" s="12" t="s">
+      <c r="B114" s="7" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="115" spans="2:2">
-      <c r="B115" s="12" t="s">
+      <c r="B115" s="7" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="116" spans="2:2">
-      <c r="B116" s="12" t="s">
+      <c r="B116" s="7" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="118" spans="2:2" ht="15.75">
-      <c r="B118" s="13" t="s">
+      <c r="B118" s="8" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="119" spans="2:2">
-      <c r="B119" s="11"/>
+      <c r="B119" s="6"/>
     </row>
     <row r="120" spans="2:2">
-      <c r="B120" s="12" t="s">
+      <c r="B120" s="7" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="121" spans="2:2">
-      <c r="B121" s="12" t="s">
+      <c r="B121" s="7" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="122" spans="2:2">
-      <c r="B122" s="12" t="s">
+      <c r="B122" s="7" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="123" spans="2:2">
-      <c r="B123" s="12" t="s">
+      <c r="B123" s="7" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="125" spans="2:2" ht="15.75">
-      <c r="B125" s="13" t="s">
+      <c r="B125" s="8" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="126" spans="2:2">
-      <c r="B126" s="11"/>
+      <c r="B126" s="6"/>
     </row>
     <row r="127" spans="2:2">
-      <c r="B127" s="12" t="s">
+      <c r="B127" s="7" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="128" spans="2:2">
-      <c r="B128" s="12" t="s">
+      <c r="B128" s="7" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="129" spans="2:2">
-      <c r="B129" s="12" t="s">
+      <c r="B129" s="7" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="130" spans="2:2">
-      <c r="B130" s="12" t="s">
+      <c r="B130" s="7" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="132" spans="2:2" ht="15.75">
-      <c r="B132" s="13" t="s">
+      <c r="B132" s="8" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="133" spans="2:2">
-      <c r="B133" s="11"/>
+      <c r="B133" s="6"/>
     </row>
     <row r="134" spans="2:2">
-      <c r="B134" s="12" t="s">
+      <c r="B134" s="7" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="135" spans="2:2">
-      <c r="B135" s="12" t="s">
+      <c r="B135" s="7" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="136" spans="2:2">
-      <c r="B136" s="12" t="s">
+      <c r="B136" s="7" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="137" spans="2:2">
-      <c r="B137" s="12" t="s">
+      <c r="B137" s="7" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="140" spans="2:2" ht="17.649999999999999">
-      <c r="B140" s="10" t="s">
+      <c r="B140" s="5" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="141" spans="2:2">
-      <c r="B141" s="11"/>
+      <c r="B141" s="6"/>
     </row>
     <row r="142" spans="2:2">
-      <c r="B142" s="12" t="s">
+      <c r="B142" s="7" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="143" spans="2:2">
-      <c r="B143" s="12" t="s">
+      <c r="B143" s="7" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="144" spans="2:2">
-      <c r="B144" s="12" t="s">
+      <c r="B144" s="7" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="145" spans="2:2">
-      <c r="B145" s="12" t="s">
+      <c r="B145" s="7" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="146" spans="2:2">
-      <c r="B146" s="12" t="s">
+      <c r="B146" s="7" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="147" spans="2:2">
-      <c r="B147" s="12" t="s">
+      <c r="B147" s="7" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="148" spans="2:2">
-      <c r="B148" s="12" t="s">
+      <c r="B148" s="7" t="s">
         <v>129</v>
       </c>
     </row>
@@ -5990,156 +5990,156 @@
       </c>
     </row>
     <row r="152" spans="2:2" ht="17.649999999999999">
-      <c r="B152" s="10" t="s">
+      <c r="B152" s="5" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="153" spans="2:2">
-      <c r="B153" s="11"/>
+      <c r="B153" s="6"/>
     </row>
     <row r="154" spans="2:2">
-      <c r="B154" s="12" t="s">
+      <c r="B154" s="7" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="155" spans="2:2">
-      <c r="B155" s="12" t="s">
+      <c r="B155" s="7" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="156" spans="2:2">
-      <c r="B156" s="12" t="s">
+      <c r="B156" s="7" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="157" spans="2:2">
-      <c r="B157" s="12" t="s">
+      <c r="B157" s="7" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="159" spans="2:2" ht="17.649999999999999">
-      <c r="B159" s="10" t="s">
+      <c r="B159" s="5" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="160" spans="2:2">
-      <c r="B160" s="11"/>
+      <c r="B160" s="6"/>
     </row>
     <row r="161" spans="2:2">
-      <c r="B161" s="12" t="s">
+      <c r="B161" s="7" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="162" spans="2:2">
-      <c r="B162" s="12" t="s">
+      <c r="B162" s="7" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="163" spans="2:2">
-      <c r="B163" s="12" t="s">
+      <c r="B163" s="7" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="164" spans="2:2">
-      <c r="B164" s="12" t="s">
+      <c r="B164" s="7" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="166" spans="2:2" ht="17.649999999999999">
-      <c r="B166" s="10" t="s">
+      <c r="B166" s="5" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="167" spans="2:2">
-      <c r="B167" s="11"/>
+      <c r="B167" s="6"/>
     </row>
     <row r="168" spans="2:2">
-      <c r="B168" s="12" t="s">
+      <c r="B168" s="7" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="169" spans="2:2">
-      <c r="B169" s="12" t="s">
+      <c r="B169" s="7" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="170" spans="2:2">
-      <c r="B170" s="12" t="s">
+      <c r="B170" s="7" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="171" spans="2:2">
-      <c r="B171" s="12" t="s">
+      <c r="B171" s="7" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="173" spans="2:2" ht="17.649999999999999">
-      <c r="B173" s="10" t="s">
+      <c r="B173" s="5" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="174" spans="2:2">
-      <c r="B174" s="11"/>
+      <c r="B174" s="6"/>
     </row>
     <row r="175" spans="2:2">
-      <c r="B175" s="12" t="s">
+      <c r="B175" s="7" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="176" spans="2:2">
-      <c r="B176" s="12" t="s">
+      <c r="B176" s="7" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="177" spans="2:2">
-      <c r="B177" s="12" t="s">
+      <c r="B177" s="7" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="178" spans="2:2">
-      <c r="B178" s="12" t="s">
+      <c r="B178" s="7" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="182" spans="2:2" ht="17.649999999999999">
-      <c r="B182" s="10" t="s">
+      <c r="B182" s="5" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="183" spans="2:2">
-      <c r="B183" s="11"/>
+      <c r="B183" s="6"/>
     </row>
     <row r="184" spans="2:2">
-      <c r="B184" s="12" t="s">
+      <c r="B184" s="7" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="185" spans="2:2">
-      <c r="B185" s="11"/>
+      <c r="B185" s="6"/>
     </row>
     <row r="186" spans="2:2">
-      <c r="B186" s="12" t="s">
+      <c r="B186" s="7" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="187" spans="2:2">
-      <c r="B187" s="11"/>
+      <c r="B187" s="6"/>
     </row>
     <row r="188" spans="2:2">
-      <c r="B188" s="12" t="s">
+      <c r="B188" s="7" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="189" spans="2:2">
-      <c r="B189" s="11"/>
+      <c r="B189" s="6"/>
     </row>
     <row r="190" spans="2:2">
-      <c r="B190" s="12" t="s">
+      <c r="B190" s="7" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="194" spans="2:2" ht="17.649999999999999">
-      <c r="B194" s="10" t="s">
+      <c r="B194" s="5" t="s">
         <v>156</v>
       </c>
     </row>
@@ -6149,499 +6149,499 @@
       </c>
     </row>
     <row r="197" spans="2:2">
-      <c r="B197" s="11"/>
+      <c r="B197" s="6"/>
     </row>
     <row r="198" spans="2:2">
-      <c r="B198" s="12" t="s">
+      <c r="B198" s="7" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="199" spans="2:2">
-      <c r="B199" s="12" t="s">
+      <c r="B199" s="7" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="200" spans="2:2">
-      <c r="B200" s="12" t="s">
+      <c r="B200" s="7" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="201" spans="2:2">
-      <c r="B201" s="12" t="s">
+      <c r="B201" s="7" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="213" spans="2:2">
-      <c r="B213" s="14" t="s">
+      <c r="B213" s="9" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="215" spans="2:2" ht="17.649999999999999">
-      <c r="B215" s="10" t="s">
+      <c r="B215" s="5" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="216" spans="2:2">
-      <c r="B216" s="11"/>
+      <c r="B216" s="6"/>
     </row>
     <row r="217" spans="2:2">
-      <c r="B217" s="12" t="s">
+      <c r="B217" s="7" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="218" spans="2:2">
-      <c r="B218" s="12" t="s">
+      <c r="B218" s="7" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="220" spans="2:2" ht="17.649999999999999">
-      <c r="B220" s="10" t="s">
+      <c r="B220" s="5" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="221" spans="2:2">
-      <c r="B221" s="11"/>
+      <c r="B221" s="6"/>
     </row>
     <row r="222" spans="2:2">
-      <c r="B222" s="12" t="s">
+      <c r="B222" s="7" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="223" spans="2:2">
-      <c r="B223" s="11"/>
+      <c r="B223" s="6"/>
     </row>
     <row r="224" spans="2:2">
-      <c r="B224" s="12" t="s">
+      <c r="B224" s="7" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="225" spans="2:2">
-      <c r="B225" s="11"/>
+      <c r="B225" s="6"/>
     </row>
     <row r="226" spans="2:2">
-      <c r="B226" s="12" t="s">
+      <c r="B226" s="7" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="227" spans="2:2">
-      <c r="B227" s="11"/>
+      <c r="B227" s="6"/>
     </row>
     <row r="228" spans="2:2">
-      <c r="B228" s="12" t="s">
+      <c r="B228" s="7" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="230" spans="2:2" ht="17.649999999999999">
-      <c r="B230" s="10" t="s">
+      <c r="B230" s="5" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="231" spans="2:2">
-      <c r="B231" s="11"/>
+      <c r="B231" s="6"/>
     </row>
     <row r="232" spans="2:2">
-      <c r="B232" s="12" t="s">
+      <c r="B232" s="7" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="234" spans="2:2" ht="17.649999999999999">
-      <c r="B234" s="10" t="s">
+      <c r="B234" s="5" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="236" spans="2:2">
-      <c r="B236" s="14" t="s">
+      <c r="B236" s="9" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="238" spans="2:2">
-      <c r="B238" s="14" t="s">
+      <c r="B238" s="9" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="239" spans="2:2">
-      <c r="B239" s="11"/>
+      <c r="B239" s="6"/>
     </row>
     <row r="240" spans="2:2">
-      <c r="B240" s="12" t="s">
+      <c r="B240" s="7" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="241" spans="2:2">
-      <c r="B241" s="12" t="s">
+      <c r="B241" s="7" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="242" spans="2:2">
-      <c r="B242" s="12" t="s">
+      <c r="B242" s="7" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="244" spans="2:2">
-      <c r="B244" s="14" t="s">
+      <c r="B244" s="9" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="245" spans="2:2">
-      <c r="B245" s="11"/>
+      <c r="B245" s="6"/>
     </row>
     <row r="246" spans="2:2">
-      <c r="B246" s="12" t="s">
+      <c r="B246" s="7" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="247" spans="2:2">
-      <c r="B247" s="12" t="s">
+      <c r="B247" s="7" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="248" spans="2:2">
-      <c r="B248" s="12" t="s">
+      <c r="B248" s="7" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="250" spans="2:2">
-      <c r="B250" s="14" t="s">
+      <c r="B250" s="9" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="251" spans="2:2">
-      <c r="B251" s="11"/>
+      <c r="B251" s="6"/>
     </row>
     <row r="252" spans="2:2">
-      <c r="B252" s="12" t="s">
+      <c r="B252" s="7" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="253" spans="2:2">
-      <c r="B253" s="12" t="s">
+      <c r="B253" s="7" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="254" spans="2:2">
-      <c r="B254" s="12" t="s">
+      <c r="B254" s="7" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="256" spans="2:2">
-      <c r="B256" s="14" t="s">
+      <c r="B256" s="9" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="257" spans="2:2">
-      <c r="B257" s="11"/>
+      <c r="B257" s="6"/>
     </row>
     <row r="258" spans="2:2">
-      <c r="B258" s="12" t="s">
+      <c r="B258" s="7" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="259" spans="2:2">
-      <c r="B259" s="12" t="s">
+      <c r="B259" s="7" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="260" spans="2:2">
-      <c r="B260" s="12" t="s">
+      <c r="B260" s="7" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="262" spans="2:2">
-      <c r="B262" s="14" t="s">
+      <c r="B262" s="9" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="263" spans="2:2">
-      <c r="B263" s="11"/>
+      <c r="B263" s="6"/>
     </row>
     <row r="264" spans="2:2">
-      <c r="B264" s="12" t="s">
+      <c r="B264" s="7" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="265" spans="2:2">
-      <c r="B265" s="12" t="s">
+      <c r="B265" s="7" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="266" spans="2:2">
-      <c r="B266" s="12" t="s">
+      <c r="B266" s="7" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="268" spans="2:2">
-      <c r="B268" s="14" t="s">
+      <c r="B268" s="9" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="269" spans="2:2">
-      <c r="B269" s="11"/>
+      <c r="B269" s="6"/>
     </row>
     <row r="270" spans="2:2">
-      <c r="B270" s="12" t="s">
+      <c r="B270" s="7" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="271" spans="2:2">
-      <c r="B271" s="12" t="s">
+      <c r="B271" s="7" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="272" spans="2:2">
-      <c r="B272" s="12" t="s">
+      <c r="B272" s="7" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="274" spans="2:2">
-      <c r="B274" s="14" t="s">
+      <c r="B274" s="9" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="275" spans="2:2">
-      <c r="B275" s="11"/>
+      <c r="B275" s="6"/>
     </row>
     <row r="276" spans="2:2">
-      <c r="B276" s="12" t="s">
+      <c r="B276" s="7" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="277" spans="2:2">
-      <c r="B277" s="12" t="s">
+      <c r="B277" s="7" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="278" spans="2:2">
-      <c r="B278" s="12" t="s">
+      <c r="B278" s="7" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="280" spans="2:2">
-      <c r="B280" s="14" t="s">
+      <c r="B280" s="9" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="281" spans="2:2">
-      <c r="B281" s="11"/>
+      <c r="B281" s="6"/>
     </row>
     <row r="282" spans="2:2">
-      <c r="B282" s="12" t="s">
+      <c r="B282" s="7" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="283" spans="2:2">
-      <c r="B283" s="12" t="s">
+      <c r="B283" s="7" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="284" spans="2:2">
-      <c r="B284" s="12" t="s">
+      <c r="B284" s="7" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="286" spans="2:2">
-      <c r="B286" s="14" t="s">
+      <c r="B286" s="9" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="287" spans="2:2">
-      <c r="B287" s="11"/>
+      <c r="B287" s="6"/>
     </row>
     <row r="288" spans="2:2">
-      <c r="B288" s="12" t="s">
+      <c r="B288" s="7" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="289" spans="2:2">
-      <c r="B289" s="12" t="s">
+      <c r="B289" s="7" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="290" spans="2:2">
-      <c r="B290" s="12" t="s">
+      <c r="B290" s="7" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="292" spans="2:2">
-      <c r="B292" s="14" t="s">
+      <c r="B292" s="9" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="293" spans="2:2">
-      <c r="B293" s="11"/>
+      <c r="B293" s="6"/>
     </row>
     <row r="294" spans="2:2">
-      <c r="B294" s="12" t="s">
+      <c r="B294" s="7" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="295" spans="2:2">
-      <c r="B295" s="12" t="s">
+      <c r="B295" s="7" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="296" spans="2:2">
-      <c r="B296" s="12" t="s">
+      <c r="B296" s="7" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="298" spans="2:2">
-      <c r="B298" s="14" t="s">
+      <c r="B298" s="9" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="299" spans="2:2">
-      <c r="B299" s="11"/>
+      <c r="B299" s="6"/>
     </row>
     <row r="300" spans="2:2">
-      <c r="B300" s="12" t="s">
+      <c r="B300" s="7" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="301" spans="2:2">
-      <c r="B301" s="12" t="s">
+      <c r="B301" s="7" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="302" spans="2:2">
-      <c r="B302" s="12" t="s">
+      <c r="B302" s="7" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="304" spans="2:2">
-      <c r="B304" s="14" t="s">
+      <c r="B304" s="9" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="305" spans="2:2">
-      <c r="B305" s="11"/>
+      <c r="B305" s="6"/>
     </row>
     <row r="306" spans="2:2">
-      <c r="B306" s="12" t="s">
+      <c r="B306" s="7" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="307" spans="2:2">
-      <c r="B307" s="12" t="s">
+      <c r="B307" s="7" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="308" spans="2:2">
-      <c r="B308" s="12" t="s">
+      <c r="B308" s="7" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="310" spans="2:2">
-      <c r="B310" s="14" t="s">
+      <c r="B310" s="9" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="311" spans="2:2">
-      <c r="B311" s="11"/>
+      <c r="B311" s="6"/>
     </row>
     <row r="312" spans="2:2">
-      <c r="B312" s="12" t="s">
+      <c r="B312" s="7" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="313" spans="2:2">
-      <c r="B313" s="12" t="s">
+      <c r="B313" s="7" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="314" spans="2:2">
-      <c r="B314" s="12" t="s">
+      <c r="B314" s="7" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="316" spans="2:2">
-      <c r="B316" s="14" t="s">
+      <c r="B316" s="9" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="317" spans="2:2">
-      <c r="B317" s="11"/>
+      <c r="B317" s="6"/>
     </row>
     <row r="318" spans="2:2">
-      <c r="B318" s="12" t="s">
+      <c r="B318" s="7" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="319" spans="2:2">
-      <c r="B319" s="12" t="s">
+      <c r="B319" s="7" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="320" spans="2:2">
-      <c r="B320" s="12" t="s">
+      <c r="B320" s="7" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="322" spans="2:2">
-      <c r="B322" s="14" t="s">
+      <c r="B322" s="9" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="323" spans="2:2">
-      <c r="B323" s="11"/>
+      <c r="B323" s="6"/>
     </row>
     <row r="324" spans="2:2">
-      <c r="B324" s="12" t="s">
+      <c r="B324" s="7" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="325" spans="2:2">
-      <c r="B325" s="12" t="s">
+      <c r="B325" s="7" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="326" spans="2:2">
-      <c r="B326" s="12" t="s">
+      <c r="B326" s="7" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="328" spans="2:2">
-      <c r="B328" s="14" t="s">
+      <c r="B328" s="9" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="329" spans="2:2">
-      <c r="B329" s="11"/>
+      <c r="B329" s="6"/>
     </row>
     <row r="330" spans="2:2">
-      <c r="B330" s="12" t="s">
+      <c r="B330" s="7" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="331" spans="2:2">
-      <c r="B331" s="12" t="s">
+      <c r="B331" s="7" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="332" spans="2:2">
-      <c r="B332" s="12" t="s">
+      <c r="B332" s="7" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="334" spans="2:2">
-      <c r="B334" s="14" t="s">
+      <c r="B334" s="9" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="335" spans="2:2">
-      <c r="B335" s="11"/>
+      <c r="B335" s="6"/>
     </row>
     <row r="336" spans="2:2">
-      <c r="B336" s="12" t="s">
+      <c r="B336" s="7" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="337" spans="2:2">
-      <c r="B337" s="12" t="s">
+      <c r="B337" s="7" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="338" spans="2:2">
-      <c r="B338" s="12" t="s">
+      <c r="B338" s="7" t="s">
         <v>238</v>
       </c>
     </row>
@@ -6659,7 +6659,8 @@
     <hyperlink ref="B33" r:id="rId2" xr:uid="{B0E6FAD6-C930-47F1-B48C-A88BEAEF2CD7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -6667,8 +6668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9E13FBE-6FDA-443F-818F-C2CD6E1BEF2F}">
   <dimension ref="B2:I65"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6736,51 +6737,51 @@
       </c>
     </row>
     <row r="14" spans="2:8">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="22" t="s">
         <v>249</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
     </row>
     <row r="15" spans="2:8">
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
     </row>
     <row r="16" spans="2:8">
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
     </row>
     <row r="17" spans="2:9">
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
     </row>
     <row r="18" spans="2:9">
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
     </row>
     <row r="20" spans="2:9">
       <c r="B20" t="s">
@@ -6792,16 +6793,16 @@
         <v>251</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="28.5">
-      <c r="E22" s="17" t="s">
+    <row r="22" spans="2:9">
+      <c r="E22" s="10" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="23" spans="2:9">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="10" t="s">
         <v>307</v>
       </c>
       <c r="F23" t="s">
@@ -6812,37 +6813,37 @@
       </c>
     </row>
     <row r="24" spans="2:9">
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="3">
         <v>6</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="H24" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="I24" s="6" t="s">
+      <c r="I24" s="3" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="17.649999999999999">
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="5" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="26" spans="2:9">
-      <c r="B26" s="11"/>
+      <c r="B26" s="6"/>
       <c r="E26" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="27" spans="2:9">
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="7" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="28" spans="2:9">
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="7" t="s">
         <v>255</v>
       </c>
       <c r="E28" t="s">
@@ -6850,274 +6851,274 @@
       </c>
     </row>
     <row r="29" spans="2:9">
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="7" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="30" spans="2:9">
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="7" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="31" spans="2:9">
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="7" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="32" spans="2:9">
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="7" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="17.649999999999999">
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="5" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="35" spans="2:4">
-      <c r="B35" s="11"/>
+      <c r="B35" s="6"/>
     </row>
     <row r="36" spans="2:4">
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="7" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="37" spans="2:4">
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="7" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="38" spans="2:4">
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="7" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="39" spans="2:4">
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="7" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="40" spans="2:4">
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="7" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="41" spans="2:4">
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="7" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="17.649999999999999">
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="5" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="44" spans="2:4">
-      <c r="B44" s="11"/>
+      <c r="B44" s="6"/>
     </row>
     <row r="45" spans="2:4">
-      <c r="B45" s="12" t="s">
+      <c r="B45" s="7" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="46" spans="2:4">
-      <c r="B46" s="12" t="s">
+      <c r="B46" s="7" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="48" spans="2:4">
-      <c r="B48" s="16"/>
-      <c r="C48" s="16" t="s">
+      <c r="B48" s="4"/>
+      <c r="C48" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="D48" s="16" t="s">
+      <c r="D48" s="4" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="49" spans="2:4">
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="C49" s="18">
+      <c r="C49" s="11">
         <v>1985</v>
       </c>
-      <c r="D49" s="18" t="s">
+      <c r="D49" s="11" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="50" spans="2:4">
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="C50" s="18">
+      <c r="C50" s="11">
         <v>1987</v>
       </c>
-      <c r="D50" s="18" t="s">
+      <c r="D50" s="11" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="51" spans="2:4">
-      <c r="B51" s="17" t="s">
+      <c r="B51" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="C51" s="18">
+      <c r="C51" s="11">
         <v>1990</v>
       </c>
-      <c r="D51" s="18" t="s">
+      <c r="D51" s="11" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="52" spans="2:4">
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="C52" s="18">
+      <c r="C52" s="11">
         <v>1992</v>
       </c>
-      <c r="D52" s="18" t="s">
+      <c r="D52" s="11" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="53" spans="2:4">
-      <c r="B53" s="17" t="s">
+      <c r="B53" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="C53" s="18">
+      <c r="C53" s="11">
         <v>1993</v>
       </c>
-      <c r="D53" s="18" t="s">
+      <c r="D53" s="11" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="54" spans="2:4">
-      <c r="B54" s="17" t="s">
+      <c r="B54" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="C54" s="18">
+      <c r="C54" s="11">
         <v>1995</v>
       </c>
-      <c r="D54" s="18" t="s">
+      <c r="D54" s="11" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="55" spans="2:4" ht="28.5">
-      <c r="B55" s="17" t="s">
+    <row r="55" spans="2:4">
+      <c r="B55" s="10" t="s">
         <v>284</v>
       </c>
-      <c r="C55" s="18">
+      <c r="C55" s="11">
         <v>1997</v>
       </c>
-      <c r="D55" s="18" t="s">
+      <c r="D55" s="11" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="56" spans="2:4">
-      <c r="B56" s="17" t="s">
+      <c r="B56" s="10" t="s">
         <v>286</v>
       </c>
-      <c r="C56" s="18">
+      <c r="C56" s="11">
         <v>1999</v>
       </c>
-      <c r="D56" s="18" t="s">
+      <c r="D56" s="11" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="57" spans="2:4">
-      <c r="B57" s="17" t="s">
+      <c r="B57" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="C57" s="18">
+      <c r="C57" s="11">
         <v>2001</v>
       </c>
-      <c r="D57" s="18" t="s">
+      <c r="D57" s="11" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="58" spans="2:4">
-      <c r="B58" s="17" t="s">
+      <c r="B58" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="C58" s="18">
+      <c r="C58" s="11">
         <v>2003</v>
       </c>
-      <c r="D58" s="18" t="s">
+      <c r="D58" s="11" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="59" spans="2:4" ht="28.5">
-      <c r="B59" s="17" t="s">
+    <row r="59" spans="2:4">
+      <c r="B59" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="C59" s="18">
+      <c r="C59" s="11">
         <v>2007</v>
       </c>
-      <c r="D59" s="18" t="s">
+      <c r="D59" s="11" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="60" spans="2:4" ht="28.5">
-      <c r="B60" s="17" t="s">
+    <row r="60" spans="2:4">
+      <c r="B60" s="10" t="s">
         <v>294</v>
       </c>
-      <c r="C60" s="18">
+      <c r="C60" s="11">
         <v>2010</v>
       </c>
-      <c r="D60" s="18" t="s">
+      <c r="D60" s="11" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="61" spans="2:4">
-      <c r="B61" s="17" t="s">
+      <c r="B61" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="C61" s="18">
+      <c r="C61" s="11">
         <v>2013</v>
       </c>
-      <c r="D61" s="18" t="s">
+      <c r="D61" s="11" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="62" spans="2:4" ht="28.5">
-      <c r="B62" s="17" t="s">
+    <row r="62" spans="2:4">
+      <c r="B62" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="C62" s="18">
+      <c r="C62" s="11">
         <v>2015</v>
       </c>
-      <c r="D62" s="18" t="s">
+      <c r="D62" s="11" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="63" spans="2:4" ht="28.5">
-      <c r="B63" s="17" t="s">
+    <row r="63" spans="2:4">
+      <c r="B63" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="C63" s="18">
+      <c r="C63" s="11">
         <v>2018</v>
       </c>
-      <c r="D63" s="18" t="s">
+      <c r="D63" s="11" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="64" spans="2:4" ht="28.5">
-      <c r="B64" s="17" t="s">
+    <row r="64" spans="2:4">
+      <c r="B64" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="C64" s="18">
+      <c r="C64" s="11">
         <v>2021</v>
       </c>
-      <c r="D64" s="18" t="s">
+      <c r="D64" s="11" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="65" spans="2:4" ht="28.5">
-      <c r="B65" s="17" t="s">
+      <c r="B65" s="10" t="s">
         <v>304</v>
       </c>
-      <c r="C65" s="18" t="s">
+      <c r="C65" s="11" t="s">
         <v>305</v>
       </c>
-      <c r="D65" s="18" t="s">
+      <c r="D65" s="11" t="s">
         <v>306</v>
       </c>
     </row>
@@ -7134,8 +7135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87BC0CBF-9B4E-40E8-B500-AF1C22111102}">
   <dimension ref="B2:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q45" sqref="Q45"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -7190,74 +7191,74 @@
       <c r="L22" t="s">
         <v>324</v>
       </c>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
-      <c r="S22" s="6"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
     </row>
     <row r="23" spans="2:19">
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="6"/>
-      <c r="S23" s="6"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
     </row>
     <row r="24" spans="2:19">
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="6"/>
-      <c r="S24" s="6"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
     </row>
     <row r="25" spans="2:19">
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
-      <c r="S25" s="6"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
     </row>
     <row r="26" spans="2:19">
-      <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
-      <c r="Q26" s="6"/>
-      <c r="R26" s="6"/>
-      <c r="S26" s="6"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
     </row>
     <row r="27" spans="2:19">
-      <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="6"/>
-      <c r="S27" s="6"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
     </row>
     <row r="28" spans="2:19" ht="14.65" thickBot="1">
-      <c r="O28" s="6"/>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="6"/>
-      <c r="R28" s="6"/>
-      <c r="S28" s="6"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
     </row>
     <row r="29" spans="2:19">
-      <c r="O29" s="19"/>
-      <c r="P29" s="19"/>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="6"/>
-      <c r="S29" s="6"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
     </row>
     <row r="30" spans="2:19">
-      <c r="O30" s="20"/>
-      <c r="P30" s="20"/>
-      <c r="Q30" s="6"/>
-      <c r="R30" s="6"/>
-      <c r="S30" s="6"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
     </row>
     <row r="31" spans="2:19" ht="14.65" thickBot="1">
-      <c r="O31" s="21"/>
-      <c r="P31" s="21"/>
-      <c r="Q31" s="6"/>
-      <c r="R31" s="6"/>
-      <c r="S31" s="6"/>
+      <c r="O31" s="14"/>
+      <c r="P31" s="14"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
     </row>
     <row r="33" spans="2:11">
       <c r="B33" t="s">
@@ -7286,7 +7287,7 @@
       <c r="F38" t="s">
         <v>332</v>
       </c>
-      <c r="I38" s="6"/>
+      <c r="I38" s="3"/>
     </row>
     <row r="39" spans="2:11">
       <c r="D39" t="s">
@@ -7298,7 +7299,7 @@
       <c r="F39" t="s">
         <v>333</v>
       </c>
-      <c r="I39" s="6"/>
+      <c r="I39" s="3"/>
     </row>
     <row r="40" spans="2:11">
       <c r="E40" t="s">
@@ -7307,19 +7308,19 @@
       <c r="F40" t="s">
         <v>336</v>
       </c>
-      <c r="H40" s="6"/>
-      <c r="I40" s="22"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
     </row>
     <row r="41" spans="2:11">
-      <c r="I41" s="6"/>
+      <c r="I41" s="3"/>
     </row>
     <row r="42" spans="2:11">
-      <c r="I42" s="6"/>
+      <c r="I42" s="3"/>
     </row>
     <row r="43" spans="2:11">
-      <c r="I43" s="6"/>
+      <c r="I43" s="3"/>
     </row>
     <row r="45" spans="2:11">
       <c r="E45" t="s">

</xml_diff>